<commit_message>
init impl for install and uninstall
</commit_message>
<xml_diff>
--- a/transfer/public/asset/xlsx/accounts.xlsx
+++ b/transfer/public/asset/xlsx/accounts.xlsx
@@ -8,7 +8,7 @@
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Account" sheetId="1" state="visible" r:id="rId3"/>
+    <sheet name="Account" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -49,17 +49,17 @@
     <r>
       <rPr>
         <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">1000 - </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">1015 - </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
         <rFont val="Noto Sans Devanagari"/>
         <family val="2"/>
         <charset val="1"/>
@@ -69,7 +69,7 @@
     <r>
       <rPr>
         <sz val="11"/>
-        <color theme="1"/>
+        <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <charset val="1"/>
@@ -81,7 +81,25 @@
     <t xml:space="preserve">خزنة غريان</t>
   </si>
   <si>
-    <t xml:space="preserve">1000</t>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">10</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">15</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">LYD</t>
@@ -90,7 +108,7 @@
     <r>
       <rPr>
         <sz val="11"/>
-        <color theme="1"/>
+        <color rgb="FF000000"/>
         <rFont val="Noto Sans Devanagari"/>
         <family val="2"/>
         <charset val="1"/>
@@ -100,7 +118,7 @@
     <r>
       <rPr>
         <sz val="11"/>
-        <color theme="1"/>
+        <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <charset val="1"/>
@@ -115,7 +133,7 @@
     <r>
       <rPr>
         <sz val="11"/>
-        <color theme="1"/>
+        <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <charset val="1"/>
@@ -125,7 +143,7 @@
     <r>
       <rPr>
         <sz val="11"/>
-        <color theme="1"/>
+        <color rgb="FF000000"/>
         <rFont val="Noto Sans Devanagari"/>
         <family val="2"/>
         <charset val="1"/>
@@ -135,7 +153,7 @@
     <r>
       <rPr>
         <sz val="11"/>
-        <color theme="1"/>
+        <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <charset val="1"/>
@@ -153,7 +171,7 @@
     <r>
       <rPr>
         <sz val="11"/>
-        <color theme="1"/>
+        <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <charset val="1"/>
@@ -163,7 +181,7 @@
     <r>
       <rPr>
         <sz val="11"/>
-        <color theme="1"/>
+        <color rgb="FF000000"/>
         <rFont val="Noto Sans Devanagari"/>
         <family val="2"/>
         <charset val="1"/>
@@ -173,7 +191,7 @@
     <r>
       <rPr>
         <sz val="11"/>
-        <color theme="1"/>
+        <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <charset val="1"/>
@@ -191,7 +209,7 @@
     <r>
       <rPr>
         <sz val="11"/>
-        <color theme="1"/>
+        <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <charset val="1"/>
@@ -201,7 +219,7 @@
     <r>
       <rPr>
         <sz val="11"/>
-        <color theme="1"/>
+        <color rgb="FF000000"/>
         <rFont val="Noto Sans Devanagari"/>
         <family val="2"/>
         <charset val="1"/>
@@ -211,7 +229,7 @@
     <r>
       <rPr>
         <sz val="11"/>
-        <color theme="1"/>
+        <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <charset val="1"/>
@@ -229,7 +247,7 @@
     <r>
       <rPr>
         <sz val="11"/>
-        <color theme="1"/>
+        <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <charset val="1"/>
@@ -239,7 +257,7 @@
     <r>
       <rPr>
         <sz val="11"/>
-        <color theme="1"/>
+        <color rgb="FF000000"/>
         <rFont val="Noto Sans Devanagari"/>
         <family val="2"/>
         <charset val="1"/>
@@ -249,7 +267,7 @@
     <r>
       <rPr>
         <sz val="11"/>
-        <color theme="1"/>
+        <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <charset val="1"/>
@@ -267,7 +285,7 @@
     <r>
       <rPr>
         <sz val="11"/>
-        <color theme="1"/>
+        <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <charset val="1"/>
@@ -277,7 +295,7 @@
     <r>
       <rPr>
         <sz val="11"/>
-        <color theme="1"/>
+        <color rgb="FF000000"/>
         <rFont val="Noto Sans Devanagari"/>
         <family val="2"/>
         <charset val="1"/>
@@ -287,7 +305,7 @@
     <r>
       <rPr>
         <sz val="11"/>
-        <color theme="1"/>
+        <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <charset val="1"/>
@@ -305,7 +323,7 @@
     <r>
       <rPr>
         <sz val="11"/>
-        <color theme="1"/>
+        <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <charset val="1"/>
@@ -315,7 +333,7 @@
     <r>
       <rPr>
         <sz val="11"/>
-        <color theme="1"/>
+        <color rgb="FF000000"/>
         <rFont val="Noto Sans Devanagari"/>
         <family val="2"/>
         <charset val="1"/>
@@ -325,7 +343,7 @@
     <r>
       <rPr>
         <sz val="11"/>
-        <color theme="1"/>
+        <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <charset val="1"/>
@@ -343,7 +361,7 @@
     <r>
       <rPr>
         <sz val="11"/>
-        <color theme="1"/>
+        <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <charset val="1"/>
@@ -353,7 +371,7 @@
     <r>
       <rPr>
         <sz val="11"/>
-        <color theme="1"/>
+        <color rgb="FF000000"/>
         <rFont val="Noto Sans Devanagari"/>
         <family val="2"/>
         <charset val="1"/>
@@ -363,7 +381,7 @@
     <r>
       <rPr>
         <sz val="11"/>
-        <color theme="1"/>
+        <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <charset val="1"/>
@@ -381,7 +399,7 @@
     <r>
       <rPr>
         <sz val="11"/>
-        <color theme="1"/>
+        <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <charset val="1"/>
@@ -391,7 +409,7 @@
     <r>
       <rPr>
         <sz val="11"/>
-        <color theme="1"/>
+        <color rgb="FF000000"/>
         <rFont val="Noto Sans Devanagari"/>
         <family val="2"/>
         <charset val="1"/>
@@ -401,7 +419,7 @@
     <r>
       <rPr>
         <sz val="11"/>
-        <color theme="1"/>
+        <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <charset val="1"/>
@@ -419,7 +437,7 @@
     <r>
       <rPr>
         <sz val="11"/>
-        <color theme="1"/>
+        <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <charset val="1"/>
@@ -429,7 +447,7 @@
     <r>
       <rPr>
         <sz val="11"/>
-        <color theme="1"/>
+        <color rgb="FF000000"/>
         <rFont val="Noto Sans Devanagari"/>
         <family val="2"/>
         <charset val="1"/>
@@ -439,7 +457,7 @@
     <r>
       <rPr>
         <sz val="11"/>
-        <color theme="1"/>
+        <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <charset val="1"/>
@@ -457,7 +475,7 @@
     <r>
       <rPr>
         <sz val="11"/>
-        <color theme="1"/>
+        <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <charset val="1"/>
@@ -467,7 +485,7 @@
     <r>
       <rPr>
         <sz val="11"/>
-        <color theme="1"/>
+        <color rgb="FF000000"/>
         <rFont val="Noto Sans Devanagari"/>
         <family val="2"/>
         <charset val="1"/>
@@ -477,7 +495,7 @@
     <r>
       <rPr>
         <sz val="11"/>
-        <color theme="1"/>
+        <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <charset val="1"/>
@@ -495,7 +513,7 @@
     <r>
       <rPr>
         <sz val="11"/>
-        <color theme="1"/>
+        <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <charset val="1"/>
@@ -505,7 +523,7 @@
     <r>
       <rPr>
         <sz val="11"/>
-        <color theme="1"/>
+        <color rgb="FF000000"/>
         <rFont val="Noto Sans Devanagari"/>
         <family val="2"/>
         <charset val="1"/>
@@ -515,7 +533,7 @@
     <r>
       <rPr>
         <sz val="11"/>
-        <color theme="1"/>
+        <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <charset val="1"/>
@@ -533,7 +551,7 @@
     <r>
       <rPr>
         <sz val="11"/>
-        <color theme="1"/>
+        <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <charset val="1"/>
@@ -543,7 +561,7 @@
     <r>
       <rPr>
         <sz val="11"/>
-        <color theme="1"/>
+        <color rgb="FF000000"/>
         <rFont val="Noto Sans Devanagari"/>
         <family val="2"/>
         <charset val="1"/>
@@ -553,7 +571,7 @@
     <r>
       <rPr>
         <sz val="11"/>
-        <color theme="1"/>
+        <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <charset val="1"/>
@@ -571,7 +589,7 @@
     <r>
       <rPr>
         <sz val="11"/>
-        <color theme="1"/>
+        <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <charset val="1"/>
@@ -581,7 +599,7 @@
     <r>
       <rPr>
         <sz val="11"/>
-        <color theme="1"/>
+        <color rgb="FF000000"/>
         <rFont val="Noto Sans Devanagari"/>
         <family val="2"/>
         <charset val="1"/>
@@ -591,7 +609,7 @@
     <r>
       <rPr>
         <sz val="11"/>
-        <color theme="1"/>
+        <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <charset val="1"/>
@@ -609,7 +627,7 @@
     <r>
       <rPr>
         <sz val="11"/>
-        <color theme="1"/>
+        <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <charset val="1"/>
@@ -619,7 +637,7 @@
     <r>
       <rPr>
         <sz val="11"/>
-        <color theme="1"/>
+        <color rgb="FF000000"/>
         <rFont val="Noto Sans Devanagari"/>
         <family val="2"/>
         <charset val="1"/>
@@ -629,7 +647,7 @@
     <r>
       <rPr>
         <sz val="11"/>
-        <color theme="1"/>
+        <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <charset val="1"/>
@@ -647,17 +665,36 @@
     <r>
       <rPr>
         <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">2000 - </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">20</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">15</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> - </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
         <rFont val="Noto Sans Devanagari"/>
         <family val="2"/>
         <charset val="1"/>
@@ -667,7 +704,7 @@
     <r>
       <rPr>
         <sz val="11"/>
-        <color theme="1"/>
+        <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <charset val="1"/>
@@ -679,13 +716,31 @@
     <t xml:space="preserve">عمولات غريان</t>
   </si>
   <si>
-    <t xml:space="preserve">2000</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">20</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">15</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
         <rFont val="Noto Sans Devanagari"/>
         <family val="2"/>
         <charset val="1"/>
@@ -695,7 +750,7 @@
     <r>
       <rPr>
         <sz val="11"/>
-        <color theme="1"/>
+        <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <charset val="1"/>
@@ -710,7 +765,7 @@
     <r>
       <rPr>
         <sz val="11"/>
-        <color theme="1"/>
+        <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <charset val="1"/>
@@ -720,7 +775,7 @@
     <r>
       <rPr>
         <sz val="11"/>
-        <color theme="1"/>
+        <color rgb="FF000000"/>
         <rFont val="Noto Sans Devanagari"/>
         <family val="2"/>
         <charset val="1"/>
@@ -730,7 +785,7 @@
     <r>
       <rPr>
         <sz val="11"/>
-        <color theme="1"/>
+        <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <charset val="1"/>
@@ -751,7 +806,7 @@
     <r>
       <rPr>
         <sz val="11"/>
-        <color theme="1"/>
+        <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <charset val="1"/>
@@ -761,7 +816,7 @@
     <r>
       <rPr>
         <sz val="11"/>
-        <color theme="1"/>
+        <color rgb="FF000000"/>
         <rFont val="Noto Sans Devanagari"/>
         <family val="2"/>
         <charset val="1"/>
@@ -771,7 +826,7 @@
     <r>
       <rPr>
         <sz val="11"/>
-        <color theme="1"/>
+        <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <charset val="1"/>
@@ -789,7 +844,7 @@
     <r>
       <rPr>
         <sz val="11"/>
-        <color theme="1"/>
+        <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <charset val="1"/>
@@ -799,7 +854,7 @@
     <r>
       <rPr>
         <sz val="11"/>
-        <color theme="1"/>
+        <color rgb="FF000000"/>
         <rFont val="Noto Sans Devanagari"/>
         <family val="2"/>
         <charset val="1"/>
@@ -809,7 +864,7 @@
     <r>
       <rPr>
         <sz val="11"/>
-        <color theme="1"/>
+        <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <charset val="1"/>
@@ -827,7 +882,7 @@
     <r>
       <rPr>
         <sz val="11"/>
-        <color theme="1"/>
+        <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <charset val="1"/>
@@ -837,7 +892,7 @@
     <r>
       <rPr>
         <sz val="11"/>
-        <color theme="1"/>
+        <color rgb="FF000000"/>
         <rFont val="Noto Sans Devanagari"/>
         <family val="2"/>
         <charset val="1"/>
@@ -847,7 +902,7 @@
     <r>
       <rPr>
         <sz val="11"/>
-        <color theme="1"/>
+        <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <charset val="1"/>
@@ -865,7 +920,7 @@
     <r>
       <rPr>
         <sz val="11"/>
-        <color theme="1"/>
+        <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <charset val="1"/>
@@ -875,7 +930,7 @@
     <r>
       <rPr>
         <sz val="11"/>
-        <color theme="1"/>
+        <color rgb="FF000000"/>
         <rFont val="Noto Sans Devanagari"/>
         <family val="2"/>
         <charset val="1"/>
@@ -885,7 +940,7 @@
     <r>
       <rPr>
         <sz val="11"/>
-        <color theme="1"/>
+        <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <charset val="1"/>
@@ -903,7 +958,7 @@
     <r>
       <rPr>
         <sz val="11"/>
-        <color theme="1"/>
+        <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <charset val="1"/>
@@ -913,7 +968,7 @@
     <r>
       <rPr>
         <sz val="11"/>
-        <color theme="1"/>
+        <color rgb="FF000000"/>
         <rFont val="Noto Sans Devanagari"/>
         <family val="2"/>
         <charset val="1"/>
@@ -923,7 +978,7 @@
     <r>
       <rPr>
         <sz val="11"/>
-        <color theme="1"/>
+        <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <charset val="1"/>
@@ -941,7 +996,7 @@
     <r>
       <rPr>
         <sz val="11"/>
-        <color theme="1"/>
+        <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <charset val="1"/>
@@ -951,7 +1006,7 @@
     <r>
       <rPr>
         <sz val="11"/>
-        <color theme="1"/>
+        <color rgb="FF000000"/>
         <rFont val="Noto Sans Devanagari"/>
         <family val="2"/>
         <charset val="1"/>
@@ -961,7 +1016,7 @@
     <r>
       <rPr>
         <sz val="11"/>
-        <color theme="1"/>
+        <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <charset val="1"/>
@@ -979,7 +1034,7 @@
     <r>
       <rPr>
         <sz val="11"/>
-        <color theme="1"/>
+        <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <charset val="1"/>
@@ -989,7 +1044,7 @@
     <r>
       <rPr>
         <sz val="11"/>
-        <color theme="1"/>
+        <color rgb="FF000000"/>
         <rFont val="Noto Sans Devanagari"/>
         <family val="2"/>
         <charset val="1"/>
@@ -999,7 +1054,7 @@
     <r>
       <rPr>
         <sz val="11"/>
-        <color theme="1"/>
+        <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <charset val="1"/>
@@ -1017,7 +1072,7 @@
     <r>
       <rPr>
         <sz val="11"/>
-        <color theme="1"/>
+        <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <charset val="1"/>
@@ -1027,7 +1082,7 @@
     <r>
       <rPr>
         <sz val="11"/>
-        <color theme="1"/>
+        <color rgb="FF000000"/>
         <rFont val="Noto Sans Devanagari"/>
         <family val="2"/>
         <charset val="1"/>
@@ -1037,7 +1092,7 @@
     <r>
       <rPr>
         <sz val="11"/>
-        <color theme="1"/>
+        <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <charset val="1"/>
@@ -1055,7 +1110,7 @@
     <r>
       <rPr>
         <sz val="11"/>
-        <color theme="1"/>
+        <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <charset val="1"/>
@@ -1065,7 +1120,7 @@
     <r>
       <rPr>
         <sz val="11"/>
-        <color theme="1"/>
+        <color rgb="FF000000"/>
         <rFont val="Noto Sans Devanagari"/>
         <family val="2"/>
         <charset val="1"/>
@@ -1075,7 +1130,7 @@
     <r>
       <rPr>
         <sz val="11"/>
-        <color theme="1"/>
+        <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <charset val="1"/>
@@ -1093,7 +1148,7 @@
     <r>
       <rPr>
         <sz val="11"/>
-        <color theme="1"/>
+        <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <charset val="1"/>
@@ -1103,7 +1158,7 @@
     <r>
       <rPr>
         <sz val="11"/>
-        <color theme="1"/>
+        <color rgb="FF000000"/>
         <rFont val="Noto Sans Devanagari"/>
         <family val="2"/>
         <charset val="1"/>
@@ -1113,7 +1168,7 @@
     <r>
       <rPr>
         <sz val="11"/>
-        <color theme="1"/>
+        <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <charset val="1"/>
@@ -1131,7 +1186,7 @@
     <r>
       <rPr>
         <sz val="11"/>
-        <color theme="1"/>
+        <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <charset val="1"/>
@@ -1141,7 +1196,7 @@
     <r>
       <rPr>
         <sz val="11"/>
-        <color theme="1"/>
+        <color rgb="FF000000"/>
         <rFont val="Noto Sans Devanagari"/>
         <family val="2"/>
         <charset val="1"/>
@@ -1151,7 +1206,7 @@
     <r>
       <rPr>
         <sz val="11"/>
-        <color theme="1"/>
+        <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <charset val="1"/>
@@ -1169,7 +1224,7 @@
     <r>
       <rPr>
         <sz val="11"/>
-        <color theme="1"/>
+        <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <charset val="1"/>
@@ -1179,7 +1234,7 @@
     <r>
       <rPr>
         <sz val="11"/>
-        <color theme="1"/>
+        <color rgb="FF000000"/>
         <rFont val="Noto Sans Devanagari"/>
         <family val="2"/>
         <charset val="1"/>
@@ -1189,7 +1244,7 @@
     <r>
       <rPr>
         <sz val="11"/>
-        <color theme="1"/>
+        <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <charset val="1"/>
@@ -1207,7 +1262,7 @@
     <r>
       <rPr>
         <sz val="11"/>
-        <color theme="1"/>
+        <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <charset val="1"/>
@@ -1217,7 +1272,7 @@
     <r>
       <rPr>
         <sz val="11"/>
-        <color theme="1"/>
+        <color rgb="FF000000"/>
         <rFont val="Noto Sans Devanagari"/>
         <family val="2"/>
         <charset val="1"/>
@@ -1227,7 +1282,7 @@
     <r>
       <rPr>
         <sz val="11"/>
-        <color theme="1"/>
+        <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <charset val="1"/>
@@ -1245,17 +1300,36 @@
     <r>
       <rPr>
         <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">3000 - </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">30</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">15</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> - </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
         <rFont val="Noto Sans Devanagari"/>
         <family val="2"/>
         <charset val="1"/>
@@ -1265,7 +1339,7 @@
     <r>
       <rPr>
         <sz val="11"/>
-        <color theme="1"/>
+        <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <charset val="1"/>
@@ -1277,13 +1351,31 @@
     <t xml:space="preserve">معلقات غريان</t>
   </si>
   <si>
-    <t xml:space="preserve">3000</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">30</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">15</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
         <rFont val="Noto Sans Devanagari"/>
         <family val="2"/>
         <charset val="1"/>
@@ -1293,19 +1385,19 @@
     <r>
       <rPr>
         <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">- A</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">- A</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <charset val="1"/>
@@ -1315,7 +1407,7 @@
     <r>
       <rPr>
         <sz val="11"/>
-        <color theme="1"/>
+        <color rgb="FF000000"/>
         <rFont val="Noto Sans Devanagari"/>
         <family val="2"/>
         <charset val="1"/>
@@ -1325,7 +1417,7 @@
     <r>
       <rPr>
         <sz val="11"/>
-        <color theme="1"/>
+        <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <charset val="1"/>
@@ -1343,7 +1435,7 @@
     <r>
       <rPr>
         <sz val="11"/>
-        <color theme="1"/>
+        <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <charset val="1"/>
@@ -1353,7 +1445,7 @@
     <r>
       <rPr>
         <sz val="11"/>
-        <color theme="1"/>
+        <color rgb="FF000000"/>
         <rFont val="Noto Sans Devanagari"/>
         <family val="2"/>
         <charset val="1"/>
@@ -1363,7 +1455,7 @@
     <r>
       <rPr>
         <sz val="11"/>
-        <color theme="1"/>
+        <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <charset val="1"/>
@@ -1381,7 +1473,7 @@
     <r>
       <rPr>
         <sz val="11"/>
-        <color theme="1"/>
+        <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <charset val="1"/>
@@ -1391,7 +1483,7 @@
     <r>
       <rPr>
         <sz val="11"/>
-        <color theme="1"/>
+        <color rgb="FF000000"/>
         <rFont val="Noto Sans Devanagari"/>
         <family val="2"/>
         <charset val="1"/>
@@ -1401,7 +1493,7 @@
     <r>
       <rPr>
         <sz val="11"/>
-        <color theme="1"/>
+        <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <charset val="1"/>
@@ -1419,7 +1511,7 @@
     <r>
       <rPr>
         <sz val="11"/>
-        <color theme="1"/>
+        <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <charset val="1"/>
@@ -1429,7 +1521,7 @@
     <r>
       <rPr>
         <sz val="11"/>
-        <color theme="1"/>
+        <color rgb="FF000000"/>
         <rFont val="Noto Sans Devanagari"/>
         <family val="2"/>
         <charset val="1"/>
@@ -1439,7 +1531,7 @@
     <r>
       <rPr>
         <sz val="11"/>
-        <color theme="1"/>
+        <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <charset val="1"/>
@@ -1457,7 +1549,7 @@
     <r>
       <rPr>
         <sz val="11"/>
-        <color theme="1"/>
+        <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <charset val="1"/>
@@ -1467,7 +1559,7 @@
     <r>
       <rPr>
         <sz val="11"/>
-        <color theme="1"/>
+        <color rgb="FF000000"/>
         <rFont val="Noto Sans Devanagari"/>
         <family val="2"/>
         <charset val="1"/>
@@ -1477,7 +1569,7 @@
     <r>
       <rPr>
         <sz val="11"/>
-        <color theme="1"/>
+        <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <charset val="1"/>
@@ -1495,7 +1587,7 @@
     <r>
       <rPr>
         <sz val="11"/>
-        <color theme="1"/>
+        <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <charset val="1"/>
@@ -1505,7 +1597,7 @@
     <r>
       <rPr>
         <sz val="11"/>
-        <color theme="1"/>
+        <color rgb="FF000000"/>
         <rFont val="Noto Sans Devanagari"/>
         <family val="2"/>
         <charset val="1"/>
@@ -1515,7 +1607,7 @@
     <r>
       <rPr>
         <sz val="11"/>
-        <color theme="1"/>
+        <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <charset val="1"/>
@@ -1533,7 +1625,7 @@
     <r>
       <rPr>
         <sz val="11"/>
-        <color theme="1"/>
+        <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <charset val="1"/>
@@ -1543,7 +1635,7 @@
     <r>
       <rPr>
         <sz val="11"/>
-        <color theme="1"/>
+        <color rgb="FF000000"/>
         <rFont val="Noto Sans Devanagari"/>
         <family val="2"/>
         <charset val="1"/>
@@ -1553,7 +1645,7 @@
     <r>
       <rPr>
         <sz val="11"/>
-        <color theme="1"/>
+        <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <charset val="1"/>
@@ -1571,7 +1663,7 @@
     <r>
       <rPr>
         <sz val="11"/>
-        <color theme="1"/>
+        <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <charset val="1"/>
@@ -1581,7 +1673,7 @@
     <r>
       <rPr>
         <sz val="11"/>
-        <color theme="1"/>
+        <color rgb="FF000000"/>
         <rFont val="Noto Sans Devanagari"/>
         <family val="2"/>
         <charset val="1"/>
@@ -1591,7 +1683,7 @@
     <r>
       <rPr>
         <sz val="11"/>
-        <color theme="1"/>
+        <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <charset val="1"/>
@@ -1609,7 +1701,7 @@
     <r>
       <rPr>
         <sz val="11"/>
-        <color theme="1"/>
+        <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <charset val="1"/>
@@ -1619,7 +1711,7 @@
     <r>
       <rPr>
         <sz val="11"/>
-        <color theme="1"/>
+        <color rgb="FF000000"/>
         <rFont val="Noto Sans Devanagari"/>
         <family val="2"/>
         <charset val="1"/>
@@ -1629,7 +1721,7 @@
     <r>
       <rPr>
         <sz val="11"/>
-        <color theme="1"/>
+        <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <charset val="1"/>
@@ -1647,7 +1739,7 @@
     <r>
       <rPr>
         <sz val="11"/>
-        <color theme="1"/>
+        <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <charset val="1"/>
@@ -1657,7 +1749,7 @@
     <r>
       <rPr>
         <sz val="11"/>
-        <color theme="1"/>
+        <color rgb="FF000000"/>
         <rFont val="Noto Sans Devanagari"/>
         <family val="2"/>
         <charset val="1"/>
@@ -1667,7 +1759,7 @@
     <r>
       <rPr>
         <sz val="11"/>
-        <color theme="1"/>
+        <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <charset val="1"/>
@@ -1685,7 +1777,7 @@
     <r>
       <rPr>
         <sz val="11"/>
-        <color theme="1"/>
+        <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <charset val="1"/>
@@ -1695,7 +1787,7 @@
     <r>
       <rPr>
         <sz val="11"/>
-        <color theme="1"/>
+        <color rgb="FF000000"/>
         <rFont val="Noto Sans Devanagari"/>
         <family val="2"/>
         <charset val="1"/>
@@ -1705,7 +1797,7 @@
     <r>
       <rPr>
         <sz val="11"/>
-        <color theme="1"/>
+        <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <charset val="1"/>
@@ -1723,7 +1815,7 @@
     <r>
       <rPr>
         <sz val="11"/>
-        <color theme="1"/>
+        <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <charset val="1"/>
@@ -1733,7 +1825,7 @@
     <r>
       <rPr>
         <sz val="11"/>
-        <color theme="1"/>
+        <color rgb="FF000000"/>
         <rFont val="Noto Sans Devanagari"/>
         <family val="2"/>
         <charset val="1"/>
@@ -1743,7 +1835,7 @@
     <r>
       <rPr>
         <sz val="11"/>
-        <color theme="1"/>
+        <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <charset val="1"/>
@@ -1761,7 +1853,7 @@
     <r>
       <rPr>
         <sz val="11"/>
-        <color theme="1"/>
+        <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <charset val="1"/>
@@ -1771,7 +1863,7 @@
     <r>
       <rPr>
         <sz val="11"/>
-        <color theme="1"/>
+        <color rgb="FF000000"/>
         <rFont val="Noto Sans Devanagari"/>
         <family val="2"/>
         <charset val="1"/>
@@ -1781,7 +1873,7 @@
     <r>
       <rPr>
         <sz val="11"/>
-        <color theme="1"/>
+        <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <charset val="1"/>
@@ -1799,7 +1891,7 @@
     <r>
       <rPr>
         <sz val="11"/>
-        <color theme="1"/>
+        <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <charset val="1"/>
@@ -1809,7 +1901,7 @@
     <r>
       <rPr>
         <sz val="11"/>
-        <color theme="1"/>
+        <color rgb="FF000000"/>
         <rFont val="Noto Sans Devanagari"/>
         <family val="2"/>
         <charset val="1"/>
@@ -1819,7 +1911,7 @@
     <r>
       <rPr>
         <sz val="11"/>
-        <color theme="1"/>
+        <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <charset val="1"/>
@@ -1841,10 +1933,10 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
@@ -1873,10 +1965,16 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF000000"/>
       <name val="Noto Sans Devanagari"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -1950,196 +2048,22 @@
 </styleSheet>
 </file>
 
-<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Office Theme">
-  <a:themeElements>
-    <a:clrScheme name="Office">
-      <a:dk1>
-        <a:srgbClr val="000000"/>
-      </a:dk1>
-      <a:lt1>
-        <a:srgbClr val="ffffff"/>
-      </a:lt1>
-      <a:dk2>
-        <a:srgbClr val="1f497d"/>
-      </a:dk2>
-      <a:lt2>
-        <a:srgbClr val="eeece1"/>
-      </a:lt2>
-      <a:accent1>
-        <a:srgbClr val="4f81bd"/>
-      </a:accent1>
-      <a:accent2>
-        <a:srgbClr val="c0504d"/>
-      </a:accent2>
-      <a:accent3>
-        <a:srgbClr val="9bbb59"/>
-      </a:accent3>
-      <a:accent4>
-        <a:srgbClr val="8064a2"/>
-      </a:accent4>
-      <a:accent5>
-        <a:srgbClr val="4bacc6"/>
-      </a:accent5>
-      <a:accent6>
-        <a:srgbClr val="f79646"/>
-      </a:accent6>
-      <a:hlink>
-        <a:srgbClr val="0000ff"/>
-      </a:hlink>
-      <a:folHlink>
-        <a:srgbClr val="800080"/>
-      </a:folHlink>
-    </a:clrScheme>
-    <a:fontScheme name="Office">
-      <a:majorFont>
-        <a:latin typeface="Cambria" pitchFamily="0" charset="1"/>
-        <a:ea typeface=""/>
-        <a:cs typeface=""/>
-      </a:majorFont>
-      <a:minorFont>
-        <a:latin typeface="Calibri" pitchFamily="0" charset="1"/>
-        <a:ea typeface=""/>
-        <a:cs typeface=""/>
-      </a:minorFont>
-    </a:fontScheme>
-    <a:fmtScheme>
-      <a:fillStyleLst>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:gradFill>
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:tint val="50000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="35000">
-              <a:schemeClr val="phClr">
-                <a:tint val="37000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:tint val="15000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="16200000" scaled="1"/>
-          <a:tileRect l="0" t="0" r="0" b="0"/>
-        </a:gradFill>
-        <a:gradFill>
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:shade val="51000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="80000">
-              <a:schemeClr val="phClr">
-                <a:shade val="93000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:shade val="94000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="16200000" scaled="0"/>
-          <a:tileRect l="0" t="0" r="0" b="0"/>
-        </a:gradFill>
-      </a:fillStyleLst>
-      <a:lnStyleLst>
-        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-          <a:prstDash val="solid"/>
-        </a:ln>
-        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
-          <a:prstDash val="solid"/>
-        </a:ln>
-        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
-          <a:prstDash val="solid"/>
-        </a:ln>
-      </a:lnStyleLst>
-      <a:effectStyleLst>
-        <a:effectStyle>
-          <a:effectLst/>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst/>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst/>
-        </a:effectStyle>
-      </a:effectStyleLst>
-      <a:bgFillStyleLst>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:gradFill>
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:tint val="40000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="40000">
-              <a:schemeClr val="phClr">
-                <a:tint val="45000"/>
-                <a:shade val="99000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:shade val="20000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:path path="circle">
-            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
-          </a:path>
-          <a:tileRect l="0" t="0" r="0" b="0"/>
-        </a:gradFill>
-        <a:gradFill>
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:tint val="80000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:shade val="30000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:path path="circle">
-            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
-          </a:path>
-          <a:tileRect l="0" t="0" r="0" b="0"/>
-        </a:gradFill>
-      </a:bgFillStyleLst>
-    </a:fmtScheme>
-  </a:themeElements>
-</a:theme>
-</file>
-
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H46"/>
+  <dimension ref="A1:H1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A28" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.59765625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.6015625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="35.58"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="1" width="10.16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="17.12"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="14.89"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="10.16"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="28.72"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="32.76"/>
@@ -2171,7 +2095,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="17.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" s="2" customFormat="true" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
         <v>8</v>
       </c>
@@ -2197,7 +2121,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="17.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" s="2" customFormat="true" ht="17.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
         <v>14</v>
       </c>
@@ -2223,7 +2147,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="17.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" s="2" customFormat="true" ht="17.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
         <v>17</v>
       </c>
@@ -2561,7 +2485,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="17.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
         <v>56</v>
       </c>
@@ -2951,7 +2875,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" customFormat="false" ht="17.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="32" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="1" t="s">
         <v>104</v>
       </c>
@@ -3341,6 +3265,9 @@
         <v>0</v>
       </c>
     </row>
+    <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511811023622047" footer="0.511811023622047"/>

</xml_diff>